<commit_message>
Added ID to contact table, Created some javascript for building the table and searching
</commit_message>
<xml_diff>
--- a/Files/Gantt.xlsx
+++ b/Files/Gantt.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Craig\Desktop\smallProject\smallProject\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185BD3D7-BD0C-478C-921C-17FC772B00F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="18135" windowHeight="7950"/>
+    <workbookView xWindow="9180" yWindow="2400" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Task</t>
   </si>
@@ -46,13 +52,16 @@
   </si>
   <si>
     <t>Note to self, update the ending date for the chart when our presentation date is assigned</t>
+  </si>
+  <si>
+    <t>Designed a Main Page for the website to use(Craig)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,9 +99,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -100,18 +106,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -119,6 +146,7 @@
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -136,6 +164,7 @@
           <c:spPr>
             <a:noFill/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$6:$A$10</c:f>
@@ -183,6 +212,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F038-47F0-938B-4A544E03FCAC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -244,6 +278,7 @@
               <a:bevelT w="63500" h="25400"/>
             </a:sp3d>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$6:$A$10</c:f>
@@ -291,8 +326,21 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F038-47F0-938B-4A544E03FCAC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
         <c:axId val="66715648"/>
         <c:axId val="66717184"/>
@@ -302,13 +350,18 @@
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="66717184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="66717184"/>
@@ -317,9 +370,12 @@
           <c:max val="44255"/>
           <c:min val="44211"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="t"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="d\-mmm" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="66715648"/>
         <c:crosses val="autoZero"/>
@@ -332,9 +388,11 @@
         <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -361,7 +419,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -422,7 +486,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -454,9 +518,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -488,6 +570,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -663,70 +763,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" ht="18.75">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -737,60 +837,71 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>44211</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>44213</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>44214</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>44215</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>44215</v>
       </c>
       <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>44220</v>
+      </c>
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
@@ -805,24 +916,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>